<commit_message>
fix excel add template
</commit_message>
<xml_diff>
--- a/src/main/resources/template.xlsx
+++ b/src/main/resources/template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Globits\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Globits\src\main\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{06188491-C6FF-4101-95E7-C0908106E292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67CC32CB-B116-43E1-B5CE-70B82368DC3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{0CEB4299-9E5E-4D1A-8FBA-666A075EF764}"/>
   </bookViews>
@@ -36,9 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t xml:space="preserve">Template Mẫu </t>
+    <t>KẾT THÚC BÁO CÁO</t>
+  </si>
+  <si>
+    <t>CÓ VẤN ĐỀ GÌ HÃY BÁO LẠI QUA EMAIL :bachh1124@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -78,7 +81,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -94,7 +97,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Chủ đề Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -410,17 +413,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A21DB7C-1959-465C-B09F-B3E17ED5B198}">
-  <dimension ref="A20"/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>